<commit_message>
Funcion para subir Indice, formato fecha, intento de escuela(faltan datos, todo comentado)
</commit_message>
<xml_diff>
--- a/ProyectoPermanencia.Presentacion/Uploads/Deuda.xlsx
+++ b/ProyectoPermanencia.Presentacion/Uploads/Deuda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Documents\Practica 2.0\Sample\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE0749B-92AA-441F-8970-CDB57BD4FEC2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0683E9EC-92E4-408A-99BF-4DD14F3652CA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
   <si>
     <t>RUT</t>
   </si>
@@ -105,7 +105,13 @@
     <t>Octubre</t>
   </si>
   <si>
-    <t>18462110K</t>
+    <t>16610707-5</t>
+  </si>
+  <si>
+    <t>18462110-K</t>
+  </si>
+  <si>
+    <t>18741199-8</t>
   </si>
 </sst>
 </file>
@@ -590,7 +596,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1301,8 +1307,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17">
-        <v>166107075</v>
+      <c r="A42" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="B42" s="12">
         <v>42972</v>
@@ -1319,7 +1325,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43" s="12">
         <v>42972</v>
@@ -1335,8 +1341,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18">
-        <v>187411998</v>
+      <c r="A44" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="B44" s="12">
         <v>43003</v>

</xml_diff>